<commit_message>
Adición de matrices iniciales Fitoplancton
</commit_message>
<xml_diff>
--- a/01_Analisis_Exploratorio/02_Datos/Biologicos/DatosP_Fitoplancton/Event_ID_EXP.PACiFICO_2021.xlsx
+++ b/01_Analisis_Exploratorio/02_Datos/Biologicos/DatosP_Fitoplancton/Event_ID_EXP.PACiFICO_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2020\01_Analisis_Exploratorio\02_Datos\Biologicos\DatosP_Fitoplancton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2021\01_Analisis_Exploratorio\02_Datos\Biologicos\DatosP_Fitoplancton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099670E9-75B9-4C7E-838B-20BE4E589BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFD740C-ECA5-4C68-BAB8-E6B01B2E09F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="2" r:id="rId1"/>
@@ -970,7 +970,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1025,6 +1025,30 @@
     <xf numFmtId="167" fontId="27" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="26" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5911,10 +5935,10 @@
   <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7775,66 +7799,66 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:22" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="12">
+      <c r="B30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="21">
         <v>44320</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="22">
         <v>0.4069444444444445</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="1" t="s">
+      <c r="E30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L30" s="15" t="str">
+      <c r="I30" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="25" t="str">
         <f>INDEX([1]Datos_Evento_Muestreo!$L$2:$L$37,MATCH(D30,[1]Datos_Evento_Muestreo!$J$2:$J$37,0))</f>
         <v>S02A</v>
       </c>
-      <c r="M30" s="5"/>
-      <c r="N30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="8" t="s">
+      <c r="M30" s="26"/>
+      <c r="N30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="S30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T30" s="11">
+      <c r="S30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="T30" s="28">
         <v>2.8</v>
       </c>
-      <c r="U30" s="11">
+      <c r="U30" s="28">
         <v>-78.11</v>
       </c>
-      <c r="V30" s="4" t="s">
+      <c r="V30" s="29" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>